<commit_message>
added multiple rooms & changed map slightly
</commit_message>
<xml_diff>
--- a/Textadventuremap.xlsx
+++ b/Textadventuremap.xlsx
@@ -29,12 +29,6 @@
     <t>Augvea</t>
   </si>
   <si>
-    <t>Weg zum Wald</t>
-  </si>
-  <si>
-    <t>Weggabelung im Wald</t>
-  </si>
-  <si>
     <t>Große Blumenwiese</t>
   </si>
   <si>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>Bärenhöhle</t>
+  </si>
+  <si>
+    <t>Waldweg</t>
+  </si>
+  <si>
+    <t>Weggabelung</t>
   </si>
 </sst>
 </file>
@@ -246,13 +246,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="24"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -338,6 +331,13 @@
       <b/>
       <sz val="20"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -519,7 +519,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -528,26 +528,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="10" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="3" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="3" xfId="9" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="11" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="13" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="3" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="7" borderId="3" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="14" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" xfId="14" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="3" xfId="14" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" xfId="12" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="5" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="3" xfId="14" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="12" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="14" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -844,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D41:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D38" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49:Q49"/>
+    <sheetView tabSelected="1" topLeftCell="G42" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="150" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -866,11 +865,11 @@
       <c r="H43" s="1"/>
       <c r="I43" s="5"/>
       <c r="J43" s="1"/>
-      <c r="K43" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L43" s="9" t="s">
-        <v>7</v>
+      <c r="K43" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="M43" s="1"/>
     </row>
@@ -879,12 +878,12 @@
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="8" t="s">
-        <v>9</v>
+      <c r="J44" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="K44" s="1"/>
-      <c r="L44" s="11" t="s">
-        <v>6</v>
+      <c r="L44" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
@@ -897,20 +896,20 @@
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="8" t="s">
-        <v>10</v>
+      <c r="J45" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="K45" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="L45" s="11" t="s">
-        <v>5</v>
+        <v>34</v>
+      </c>
+      <c r="L45" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
-      <c r="P45" s="17" t="s">
-        <v>26</v>
+      <c r="P45" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="Q45" s="1"/>
     </row>
@@ -918,62 +917,62 @@
       <c r="D46" s="1"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>22</v>
+      <c r="G46" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="4"/>
       <c r="K46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L46" s="14" t="s">
         <v>1</v>
-      </c>
-      <c r="L46" s="15" t="s">
-        <v>3</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="P46" s="17" t="s">
-        <v>25</v>
+      <c r="O46" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P46" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
     </row>
     <row r="47" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E47" s="5"/>
-      <c r="F47" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" s="19" t="s">
+      <c r="F47" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="I47" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J47" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K47" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K47" s="13" t="s">
         <v>0</v>
       </c>
       <c r="L47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M47" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N47" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M47" s="12" t="s">
+      <c r="O47" s="16" t="s">
         <v>12</v>
-      </c>
-      <c r="N47" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="O47" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
@@ -981,17 +980,17 @@
     <row r="48" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
-      <c r="G48" s="20" t="s">
-        <v>19</v>
+      <c r="G48" s="18" t="s">
+        <v>17</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="4"/>
       <c r="K48" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L48" s="23" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="L48" s="21" t="s">
+        <v>25</v>
       </c>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
@@ -1001,23 +1000,23 @@
     <row r="49" spans="5:15" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E49" s="1"/>
       <c r="F49" s="5"/>
-      <c r="G49" s="21" t="s">
-        <v>20</v>
+      <c r="G49" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="5"/>
       <c r="K49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L49" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="M49" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L49" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="M49" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="N49" s="27" t="s">
-        <v>34</v>
+      <c r="N49" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="O49" s="1"/>
     </row>
@@ -1029,11 +1028,11 @@
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
       <c r="L50" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="M50" s="1"/>
-      <c r="N50" s="8" t="s">
-        <v>32</v>
+      <c r="N50" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="O50" s="1"/>
     </row>
@@ -1043,11 +1042,11 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
-      <c r="K51" s="24"/>
+      <c r="K51" s="22"/>
       <c r="L51" s="5"/>
       <c r="M51" s="1"/>
-      <c r="N51" s="10" t="s">
-        <v>33</v>
+      <c r="N51" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="O51" s="1"/>
     </row>

</xml_diff>

<commit_message>
added 5 new rooms and edited map
</commit_message>
<xml_diff>
--- a/Textadventuremap.xlsx
+++ b/Textadventuremap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Augvea</t>
   </si>
@@ -129,13 +129,28 @@
   </si>
   <si>
     <t>Weggabelung</t>
+  </si>
+  <si>
+    <t>Krähenhort</t>
+  </si>
+  <si>
+    <t>Große Düne</t>
+  </si>
+  <si>
+    <t>Met'Schall-Wüste</t>
+  </si>
+  <si>
+    <t>Apfelwiese</t>
+  </si>
+  <si>
+    <t>Öder Morast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,13 +176,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -225,29 +233,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="24"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="24"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="24"/>
-      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -255,7 +275,37 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,87 +313,18 @@
     <font>
       <b/>
       <sz val="22"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="26"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="26"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +392,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -502,54 +489,61 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="9" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="3" xfId="9" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="11" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="13" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="12" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="2" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" xfId="14" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" xfId="14" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="11" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="3" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="3" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" xfId="14" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="3" xfId="14" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="12" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="5" xfId="8" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="10" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="14" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" xfId="14" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="10" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="13" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="14" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" xfId="13" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="13" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="16">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - Accent4" xfId="15" builtinId="42"/>
     <cellStyle name="20% - Accent6" xfId="13" builtinId="50"/>
     <cellStyle name="40% - Accent1" xfId="11" builtinId="31"/>
     <cellStyle name="60% - Accent6" xfId="14" builtinId="52"/>
@@ -843,13 +837,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D41:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G42" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="F42" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="150" customHeight="1" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="16384" width="30.7109375" style="3"/>
+    <col min="1" max="16384" width="30.7109375" style="4"/>
   </cols>
   <sheetData>
     <row r="41" spans="4:18" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
@@ -857,125 +851,129 @@
     </row>
     <row r="42" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="H42" s="5"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
     </row>
     <row r="43" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G43" s="5"/>
-      <c r="H43" s="1"/>
+      <c r="H43" s="6"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="10" t="s">
+      <c r="J43" s="6"/>
+      <c r="K43" s="7" t="s">
         <v>6</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M43" s="1"/>
+      <c r="M43" s="6"/>
     </row>
     <row r="44" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F44" s="1"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="7" t="s">
+      <c r="J44" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="10" t="s">
+      <c r="K44" s="6"/>
+      <c r="L44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
     </row>
     <row r="45" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="27" t="s">
+        <v>20</v>
+      </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="7" t="s">
+      <c r="J45" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K45" s="7" t="s">
+      <c r="K45" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L45" s="10" t="s">
+      <c r="L45" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="16" t="s">
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="Q45" s="1"/>
+      <c r="Q45" s="6"/>
     </row>
     <row r="46" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="D46" s="1"/>
+      <c r="D46" s="6"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="14" t="s">
-        <v>20</v>
+      <c r="H46" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="I46" s="5"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="3" t="s">
+      <c r="J46" s="12"/>
+      <c r="K46" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L46" s="14" t="s">
+      <c r="L46" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="16" t="s">
+      <c r="M46" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="N46" s="6"/>
+      <c r="O46" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="P46" s="16" t="s">
+      <c r="P46" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
     </row>
     <row r="47" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E47" s="5"/>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="G47" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H47" s="26" t="s">
+      <c r="H47" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J47" s="12" t="s">
+      <c r="J47" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="K47" s="13" t="s">
+      <c r="K47" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L47" s="3" t="s">
+      <c r="L47" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M47" s="11" t="s">
+      <c r="M47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N47" s="15" t="s">
+      <c r="N47" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="O47" s="16" t="s">
+      <c r="O47" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
     </row>
     <row r="48" spans="4:18" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" s="5"/>
@@ -983,82 +981,88 @@
       <c r="G48" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="2" t="s">
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L48" s="21" t="s">
+      <c r="L48" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
+      <c r="M48" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="N48" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="O48" s="6"/>
+      <c r="P48" s="6"/>
     </row>
     <row r="49" spans="5:15" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E49" s="1"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="5"/>
-      <c r="G49" s="19" t="s">
+      <c r="G49" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
       <c r="J49" s="5"/>
-      <c r="K49" s="3" t="s">
+      <c r="K49" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="L49" s="24" t="s">
+      <c r="L49" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="M49" s="7" t="s">
+      <c r="M49" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N49" s="25" t="s">
+      <c r="N49" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="O49" s="1"/>
-    </row>
-    <row r="50" spans="5:15" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="O49" s="6"/>
+    </row>
+    <row r="50" spans="5:15" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
-      <c r="L50" s="6" t="s">
+      <c r="L50" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="M50" s="1"/>
-      <c r="N50" s="7" t="s">
+      <c r="M50" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N50" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="O50" s="1"/>
+      <c r="O50" s="6"/>
     </row>
     <row r="51" spans="5:15" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F51" s="5"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="22"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="25"/>
       <c r="L51" s="5"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="9" t="s">
+      <c r="M51" s="6"/>
+      <c r="N51" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="O51" s="1"/>
+      <c r="O51" s="6"/>
     </row>
     <row r="52" spans="5:15" ht="150" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
       <c r="L52" s="5"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
     </row>
     <row r="53" spans="5:15" ht="150" customHeight="1" thickTop="1" x14ac:dyDescent="0.5"/>
   </sheetData>

</xml_diff>